<commit_message>
update 22:24 - 30/08/2024 - all run ok
</commit_message>
<xml_diff>
--- a/news_data.xlsx
+++ b/news_data.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="news" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,19 +451,29 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>search_phrase_count</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>contains_money</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>image_name</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Russia's Putin to visit ICC member Mongolia despite arrest warrant ...</t>
+          <t>Judge orders 'immediate suspension' of X in Brazil | Social Media ...</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>6 hours ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... More from News. Several killed in Israeli attack on Gaza medical convoy ...</t>
+          <t>4 hours ago ... The move is the latest chapter in an ongoing feud between a Supreme Court judge in Brazil and Elon Musk ... Economy|Social Media. Judge orders ' ...</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -471,19 +481,27 @@
           <t>30 Aug 2024</t>
         </is>
       </c>
-      <c r="D2" t="b">
-        <v>0</v>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Imagem_01.jpg</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Israeli forces inflict major damage in occupied West Bank | Israel ...</t>
+          <t>Russia's Putin to visit ICC member Mongolia despite arrest warrant ...</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1 minute ago ... Much of Tulkarem in the occupied West Bank has reportedly lost water access due to an Israeli military assault.</t>
+          <t>13 hours ago ... Last year, he skipped a summit of the BRICS bloc of developing economies, which includes Brazil, Russia, India, China and South Africa, in ...</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -491,19 +509,27 @@
           <t>30 Aug 2024</t>
         </is>
       </c>
-      <c r="D3" t="b">
-        <v>0</v>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Imagem_02.jpg</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Diary of a Jenin family, hiding in the kitchen from Israel's assault ...</t>
+          <t>Pakistan's storm Asna: Legend of the Karachi saint who can 'stop ...</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3 hours ago ... From her kitchen, Saja Bawaqneh, 29, recounts the first day of Israel's raid into the West Bank's Jenin refugee camp ... Economy · Climate Crisis ...</t>
+          <t>10 hours ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... Judge orders 'immediate suspension' of X in Brazil. Elon Musk has ...</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -511,19 +537,27 @@
           <t>30 Aug 2024</t>
         </is>
       </c>
-      <c r="D4" t="b">
-        <v>0</v>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Imagem_03.jpg</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Israel's war on Gaza live: Israel leaves bodies in wake of Khan ...</t>
+          <t>More than $200m: How Kamala Harris is winning the small donors ...</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3 hours ago ... Civil defence in says it is working to recover people killed in a 22-day Israeli army operation in eastern Khan Younis.</t>
+          <t>11 hours ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... Judge orders 'immediate suspension' of X in Brazil. Elon Musk has ...</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -531,19 +565,27 @@
           <t>30 Aug 2024</t>
         </is>
       </c>
-      <c r="D5" t="b">
-        <v>0</v>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Imagem_04.jpg</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Five key takeaways from Kamala Harris, Tim Walz's first major TV ...</t>
+          <t>France's Macron defends giving citizenship to Telegram CEO Pavel ...</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>13 hours ago ... “What I've seen is that we can grow and we can increase a thriving clean energy economy without banning fracking. ... Israel's defence and ...</t>
+          <t>23 hours ago ... More from Economy. Judge orders 'immediate suspension' of X in Brazil. Elon Musk has denounced as censorship orders by a judge in Brazil to ...</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -551,108 +593,1192 @@
           <t>30 Aug 2024</t>
         </is>
       </c>
-      <c r="D6" t="b">
-        <v>0</v>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Imagem_05.jpg</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>The Take: Beyond Gaza – Israel's military escalation in the West ...</t>
+          <t>Ahead of key interview, five questions Kamala Harris hasn't ...</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>13 hours ago ... Israeli soldiers are conducting a major assault in the occupied West Bank, targeting Jenin, Tulkarem and Far'a camp.</t>
+          <t>1 day ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... Judge orders 'immediate suspension' of X in Brazil. Elon Musk has ...</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>29 Aug 2024</t>
-        </is>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
+          <t>30 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Imagem_06.jpg</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Libya's central bank chief flees country over militia threats: Report ...</t>
+          <t>Brazil's top court threatens to ban Elon Musk's X | Social Media | Al ...</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7 hours ago ... Al-Kabir had accused the prime minister of “overspending and painting a misleadingly 'rosy' picture of the economy in his speeches”. Critics ...</t>
+          <t>2 days ago ... Economy|Social Media. Brazil's top court threatens to ban Elon Musk's X ... Brazil's top court has threatened to ban X unless its billionaire ...</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>30 Aug 2024</t>
-        </is>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
+          <t>29 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Imagem_07.jpg</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Several killed in Israeli attack on Gaza medical convoy, aid group says</t>
+          <t>South Korea arrests battery maker CEO over fire that killed 23 ...</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1 hour ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... Israel claimed without immediate evidence that it opened fire after ...</t>
+          <t>2 days ago ... Sagging exports and private consumption see Asia's fourth-largest economy contract for first time in 2-1/2 years. ... More from Economy. Brazil's ...</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>30 Aug 2024</t>
-        </is>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
+          <t>29 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Imagem_08.jpg</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Destruction after Israeli raid on occupied West Bank refugee camp ...</t>
+          <t>Russia lashes out against 'terrorist' incursion in Kursk, pulls back ...</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7 hours ago ... Al Jazeera's Nida Ibrahim is in Nur Shams refugee camp where Israeli forces have caused significant damage.</t>
+          <t>1 day ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... Judge orders 'immediate suspension' of X in Brazil. Elon Musk has ...</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>30 Aug 2024</t>
-        </is>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
+          <t>29 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Imagem_09.jpg</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>France's Macron defends giving citizenship to Telegram CEO Pavel ...</t>
+          <t>Brazil judge blocks Starlink accounts as X suspension deadline ...</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>15 hours ago ... Economy|Social Media. France's Macron defends giving citizenship to ... Khan Younis a 'wasteland' after Israeli army exit, as 9 bodies found so ...</t>
+          <t>1 day ago ... Earlier this month, X announced it would close operations and fire its staff in Latin America's largest economy due to what it called “ ...</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>30 Aug 2024</t>
-        </is>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
+          <t>29 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Imagem_10.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Colourful, joyous opening ceremony kickstarts Paralympic Games ...</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2 days ago ... Some delegations were huge – more than 250 athletes from Brazil – and some were tiny – less than a handful from Barbados and just three from ...</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>29 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Imagem_11.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>In Venezuela's diaspora, protests erupt against Maduro's contested ...</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1 day ago ... ... economy. Meanwhile, the governments of Peru, Ecuador, Costa Rica ... Brazil-based humanitarian organisation that has advocated for election ...</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>29 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Imagem_12.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>The Paris Paralympics open in blaze of colour | Paris Olympics 2024 ...</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2 days ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... Brazil lead their contingent during the opening ceremony. [Andrew ...</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>28 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Imagem_13.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>A dangerous precedent? Telegram CEO Pavel Durov's arrest stokes ...</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>3 days ago ... More from Economy. France's Macron defends giving ... A Brazilian judge had asked Elon Musk to name a legal representative for X in Brazil ...</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>28 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Imagem_14.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Drug dealers to Putin critics: Behind Pavel Durov's rare Telegram ...</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>3 days ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... Brazil judge blocks Starlink accounts as X suspension deadline looms.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>28 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Imagem_15.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Russia-Ukraine war: List of key events, day 915 | Russia-Ukraine ...</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>3 days ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... Brazil and South Africa. “They have maintained communication with ...</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>28 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Imagem_16.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Dozens missing in Yemen floods, risk of cholera outbreak rises ...</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3 days ago ... Economy · Climate Crisis · Investigations · Interactives ... A Brazilian judge had asked Elon Musk to name a legal representative for X in Brazil ...</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>29 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Imagem_17.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Elon Musk's X tweaks chatbot after warning over US election ...</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4 days ago ... Economy|US Election 2024. Elon Musk's X tweaks chatbot after warning ... Elon Musk's X to shut operations in Brazil amid bitter legal fight.</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>27 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Imagem_18.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Australia caps international student numbers amid discontent over ...</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>4 days ago ... More from Economy. Brazil's top court threatens to ban Elon Musk's X. X owner Elon Musk listens to a question at a conference on March 9, 2020 ...</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>27 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Imagem_19.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Brazil forms committee to oversee probe into plane crash that killed ...</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>3 days ago ... Panel expected to call on several key figures in bid to prevent repeat of deadly crash north of Sao Paulo.</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>27 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Imagem_20.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>All to know about Paralympic Games Paris 2024: Schedule, events ...</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>4 days ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures · Science ... Alana Maldonado (Brazil): Para judo; Patrick Anderson (Canada): ...</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>27 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Imagem_21.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>The Take: The fallacies of Israel's 'Octopus Doctrine' | News | Al ...</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5 days ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... The Take: Inside Brazil's abortion culture wars. end of list. In this ...</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>26 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Imagem_22.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Why is Belarus amassing troops along its border with Ukraine ...</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>4 days ago ... What is Belarus's position on the Russia-Ukraine war? Belarus has maintained close political and economic relations with Russia since its ...</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>26 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Imagem_23.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Who is Telegram founder Pavel Durov? All to know about his arrest ...</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>4 days ago ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... In 2016, a senior Facebook executive was arrested in Brazil after ...</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>26 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Imagem_24.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Kamala Harris sets fundraising record with $540m after DNC | US ...</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>5 days ago ... Can Kamala Harris help boost the world's largest economy? The ... More from News. Judge orders 'immediate suspension' of X in Brazil.</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>26 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Imagem_25.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>More than 70 killed in multiple armed attacks in Pakistan's ...</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>4 days ago ... Economy · Climate Crisis · Investigations · Interactives ... A Brazilian judge had asked Elon Musk to name a legal representative for X in Brazil ...</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>26 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Imagem_26.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Australia gives workers right to ignore bosses' after-hours calls ...</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>5 days ago ... ... economy at the worst possible time,” Black told Al Jazeera. “Our ... Brazil's top court threatens to ban Elon Musk's X. X owner Elon ...</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>26 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Imagem_27.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Canada follows US, imposes 100% tariff on EVs imported from ...</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>4 days ago ... Economy|Trade War. Canada follows US, imposes 100% tariff on EVs ... More from Economy. Brazil's top court threatens to ban Elon Musk's X.</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>26 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Imagem_28.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Airlines suspend flights over clashes between Israel and Hezbollah ...</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>5 days ago ... More from Economy. Brazil's top court threatens to ban Elon Musk's X. X owner Elon Musk listens to a question at a conference on March 9, 2020 ...</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>26 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Imagem_29.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Police say 20 abducted Nigerian medical students freed | Crime ...</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>7 days ago ... Economy · Climate Crisis · Investigations · Interactives ... A Brazilian judge had asked Elon Musk to name a legal representative for X in Brazil ...</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>24 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Imagem_30.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>ICC prosecutor urges judges to rule on warrants for Israeli, Hamas ...</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>7 days ago ... Gaza war extends toll on Israel's economy. end of list. Khan had ... Judge orders 'immediate suspension' of X in Brazil. Elon Musk has ...</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>24 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Imagem_31.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Panda Meng Meng gives birth to second set of twins at Berlin Zoo ...</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Aug 22, 2024 ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... A Brazilian Sharpnose Shark (Rhizoprionodon Lalandii) is being analysed ...</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>23 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Imagem_32.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CN workers to strike Monday, vow to fight Canada move to end rail ...</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Aug 22, 2024 ... The union representing workers at the Canadian National Railway (CN) says they will strike next week, in a new threat to the economy after ...</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>23 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Imagem_33.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Nepal lifts TikTok ban after blocking app over 'social harmony ...</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Aug 22, 2024 ... More from Economy. Judge orders 'immediate suspension' of X in Brazil. Elon Musk has denounced as censorship orders by a judge in Brazil to ...</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>23 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Imagem_34.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>US Fed's Powell says 'time has come' to lower interest rates ...</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Aug 22, 2024 ... ... economy was starting to slow down [File: Nam Y Huh/AP Photo] ... Brazil's top court threatens to ban Elon Musk's X. X owner Elon Musk ...</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>23 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Imagem_35.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Transgender woman's ban from female-only app discriminatory ...</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Aug 22, 2024 ... More from Economy. France's Macron defends giving citizenship to ... Brazil's top court threatens to ban Elon Musk's X. X owner Elon Musk ...</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>23 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Imagem_36.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Gaza war extends toll on Israel's economy | Israel-Palestine conflict ...</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Aug 22, 2024 ... Brazil's top court threatens to ban Elon Musk's X. X owner Elon Musk listens to a question at a conference on March 9, 2020. South Korea ...</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>23 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Imagem_37.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>The Take: How the murder of a doctor reignited India's rage against ...</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Aug 21, 2024 ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... The Take: Inside Brazil's abortion culture wars. list 3 of 4. The Take ...</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>22 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Imagem_38.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Robert F Kennedy Jr to drop US presidential bid, back Trump ...</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Aug 21, 2024 ... Can Kamala Harris help boost the world's largest economy? ... A Brazilian judge had asked Elon Musk to name a legal representative for X in Brazil ...</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>22 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Imagem_39.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Andrew and Tristan Tate detained in Romania in new trafficking ...</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Aug 21, 2024 ... Economy|Crime. Andrew and Tristan Tate detained in Romania in ... Brazil's top court threatens to ban Elon Musk's X. X owner Elon Musk ...</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>22 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Imagem_40.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Indonesia and Australia finalise 'significant' defence pact | Military ...</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Aug 19, 2024 ... ... economy, food security, agriculture, and curbing ... A Brazilian judge had asked Elon Musk to name a legal representative for X in Brazil ...</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>20 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Imagem_41.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>US orders inspections of Boeing 787 planes following midair plunge ...</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Aug 19, 2024 ... More from Economy. Brazil's top court threatens to ban Elon Musk's X. X owner Elon Musk listens to a question at a conference on March 9, 2020 ...</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>20 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Imagem_42.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Philippines agrees to host Afghans awaiting resettlement in US ...</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Aug 19, 2024 ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... The Take: Inside Brazil's abortion culture wars. end of list. “The ...</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>20 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Imagem_43.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Trump Media shares hit record low as race tightens for former US ...</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Aug 19, 2024 ... Economy|Donald Trump. Trump Media shares hit record low as race ... Brazil's top court threatens to ban Elon Musk's X. X owner Elon Musk ...</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>20 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Imagem_44.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Nicaragua bans 1,500 NGOs in latest crackdown against civil ...</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Aug 18, 2024 ... Economy · Climate ... Nicaragua joins Mexico in severing ties with Quito, while Brazil said the embassy raid is a clear violation of law.</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>19 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Imagem_45.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>The unlikely origins of some of the world's favourite foods | Food ...</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Aug 17, 2024 ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... Brazil. According to food historians, during the Japanese colonial ...</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>20 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Imagem_46.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Trump's control over party in focus as Republicans convene, post ...</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Jul 13, 2024 ... Economy · Climate Crisis · Investigations · Interactives · In Pictures ... Judge orders 'immediate suspension' of X in Brazil. Elon Musk has ...</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>26 Aug 2024</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" t="b">
+        <v>0</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Imagem_47.jpg</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>